<commit_message>
Moved Battle Order to Util
</commit_message>
<xml_diff>
--- a/cards.xlsx
+++ b/cards.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AustinWilliams\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AustinWilliams\PycharmProjects\SPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6500EED-2D01-4690-91C1-DAC1D5FD1E69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F24882E2-58F2-45B4-B742-1515A679CFBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9650" yWindow="540" windowWidth="14400" windowHeight="9240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4990" yWindow="1350" windowWidth="14400" windowHeight="9240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="81">
   <si>
     <t>Card</t>
   </si>
@@ -137,6 +137,132 @@
   </si>
   <si>
     <t>Spark Pixies</t>
+  </si>
+  <si>
+    <t>Pyre</t>
+  </si>
+  <si>
+    <t>summoner</t>
+  </si>
+  <si>
+    <t>speed+</t>
+  </si>
+  <si>
+    <t>Malric Inferno</t>
+  </si>
+  <si>
+    <t>Pirate Captain</t>
+  </si>
+  <si>
+    <t>water</t>
+  </si>
+  <si>
+    <t>Spineback Turtle</t>
+  </si>
+  <si>
+    <t>Crustacean King</t>
+  </si>
+  <si>
+    <t>Sabre Shark</t>
+  </si>
+  <si>
+    <t>Feasting Seaweed</t>
+  </si>
+  <si>
+    <t>Albatross</t>
+  </si>
+  <si>
+    <t>Tortisian Fighter</t>
+  </si>
+  <si>
+    <t>Sniping Narwhal</t>
+  </si>
+  <si>
+    <t>Alric Stormbringer</t>
+  </si>
+  <si>
+    <t>Medusa</t>
+  </si>
+  <si>
+    <t>Water Elemental</t>
+  </si>
+  <si>
+    <t>Frozen Soldier</t>
+  </si>
+  <si>
+    <t>Ice Pixie</t>
+  </si>
+  <si>
+    <t>Giant Squid</t>
+  </si>
+  <si>
+    <t>Serpent of Eld</t>
+  </si>
+  <si>
+    <t>Bortus</t>
+  </si>
+  <si>
+    <t>magic</t>
+  </si>
+  <si>
+    <t>tank heal</t>
+  </si>
+  <si>
+    <t>magic+</t>
+  </si>
+  <si>
+    <t>dodge</t>
+  </si>
+  <si>
+    <t>magic-</t>
+  </si>
+  <si>
+    <t>Peaceful Giant</t>
+  </si>
+  <si>
+    <t>Grumpy Dwarf</t>
+  </si>
+  <si>
+    <t>Elven Cutthroat</t>
+  </si>
+  <si>
+    <t>Centaur</t>
+  </si>
+  <si>
+    <t>Elven Defender</t>
+  </si>
+  <si>
+    <t>Horny Toad</t>
+  </si>
+  <si>
+    <t>Mantoid</t>
+  </si>
+  <si>
+    <t>Parasitic Growth</t>
+  </si>
+  <si>
+    <t>Cocatrice</t>
+  </si>
+  <si>
+    <t>Cyclops</t>
+  </si>
+  <si>
+    <t>Enchanted Pixie</t>
+  </si>
+  <si>
+    <t>Elven Mystic</t>
+  </si>
+  <si>
+    <t>Goblin Chariot</t>
+  </si>
+  <si>
+    <t>Tower Griffin</t>
+  </si>
+  <si>
+    <t>neutral</t>
+  </si>
+  <si>
+    <t>melee+</t>
   </si>
 </sst>
 </file>
@@ -538,15 +664,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20.26953125" customWidth="1"/>
+    <col min="2" max="2" width="10.7265625" customWidth="1"/>
     <col min="6" max="6" width="16.08984375" customWidth="1"/>
     <col min="10" max="10" width="11.1796875" customWidth="1"/>
   </cols>
@@ -1028,6 +1155,982 @@
         <v>22</v>
       </c>
     </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18">
+        <v>2</v>
+      </c>
+      <c r="H18">
+        <v>3</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>6</v>
+      </c>
+      <c r="I19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>2</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21">
+        <v>3</v>
+      </c>
+      <c r="H21">
+        <v>2</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22">
+        <v>4</v>
+      </c>
+      <c r="E22">
+        <v>2</v>
+      </c>
+      <c r="F22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>2</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24">
+        <v>4</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="F24" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>3</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25">
+        <v>5</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="F25" t="s">
+        <v>21</v>
+      </c>
+      <c r="G25">
+        <v>2</v>
+      </c>
+      <c r="H25">
+        <v>4</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27">
+        <v>4</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27" t="s">
+        <v>60</v>
+      </c>
+      <c r="G27">
+        <v>2</v>
+      </c>
+      <c r="H27">
+        <v>3</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" t="s">
+        <v>44</v>
+      </c>
+      <c r="D28">
+        <v>5</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="F28" t="s">
+        <v>21</v>
+      </c>
+      <c r="G28">
+        <v>4</v>
+      </c>
+      <c r="H28">
+        <v>4</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" t="s">
+        <v>44</v>
+      </c>
+      <c r="D29">
+        <v>6</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="F29" t="s">
+        <v>12</v>
+      </c>
+      <c r="G29">
+        <v>2</v>
+      </c>
+      <c r="H29">
+        <v>3</v>
+      </c>
+      <c r="I29">
+        <v>5</v>
+      </c>
+      <c r="J29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" t="s">
+        <v>44</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30" t="s">
+        <v>60</v>
+      </c>
+      <c r="G30">
+        <v>3</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D31">
+        <v>5</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+      <c r="F31" t="s">
+        <v>21</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>4</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" t="s">
+        <v>44</v>
+      </c>
+      <c r="D32">
+        <v>7</v>
+      </c>
+      <c r="E32">
+        <v>3</v>
+      </c>
+      <c r="F32" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32">
+        <v>4</v>
+      </c>
+      <c r="H32">
+        <v>5</v>
+      </c>
+      <c r="I32">
+        <v>2</v>
+      </c>
+      <c r="J32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" t="s">
+        <v>44</v>
+      </c>
+      <c r="D33">
+        <v>3</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" t="s">
+        <v>79</v>
+      </c>
+      <c r="D34">
+        <v>5</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="H34">
+        <v>8</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" t="s">
+        <v>79</v>
+      </c>
+      <c r="D35">
+        <v>4</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35" t="s">
+        <v>12</v>
+      </c>
+      <c r="G35">
+        <v>2</v>
+      </c>
+      <c r="H35">
+        <v>2</v>
+      </c>
+      <c r="I35">
+        <v>1</v>
+      </c>
+      <c r="J35" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" t="s">
+        <v>79</v>
+      </c>
+      <c r="D36">
+        <v>3</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36">
+        <v>3</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" t="s">
+        <v>79</v>
+      </c>
+      <c r="D37">
+        <v>4</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37" t="s">
+        <v>21</v>
+      </c>
+      <c r="G37">
+        <v>3</v>
+      </c>
+      <c r="H37">
+        <v>4</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="J37" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>69</v>
+      </c>
+      <c r="B38" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" t="s">
+        <v>79</v>
+      </c>
+      <c r="D38">
+        <v>8</v>
+      </c>
+      <c r="E38">
+        <v>2</v>
+      </c>
+      <c r="F38" t="s">
+        <v>12</v>
+      </c>
+      <c r="G38">
+        <v>2</v>
+      </c>
+      <c r="H38">
+        <v>8</v>
+      </c>
+      <c r="I38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>70</v>
+      </c>
+      <c r="B39" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" t="s">
+        <v>79</v>
+      </c>
+      <c r="D39">
+        <v>3</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39" t="s">
+        <v>12</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39">
+        <v>2</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>71</v>
+      </c>
+      <c r="B40" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" t="s">
+        <v>79</v>
+      </c>
+      <c r="D40">
+        <v>6</v>
+      </c>
+      <c r="E40">
+        <v>2</v>
+      </c>
+      <c r="F40" t="s">
+        <v>21</v>
+      </c>
+      <c r="G40">
+        <v>2</v>
+      </c>
+      <c r="H40">
+        <v>5</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>72</v>
+      </c>
+      <c r="B41" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" t="s">
+        <v>79</v>
+      </c>
+      <c r="D41">
+        <v>4</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41" t="s">
+        <v>12</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+      <c r="H41">
+        <v>2</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B42" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" t="s">
+        <v>79</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42" t="s">
+        <v>12</v>
+      </c>
+      <c r="G42">
+        <v>3</v>
+      </c>
+      <c r="H42">
+        <v>2</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>74</v>
+      </c>
+      <c r="B43" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" t="s">
+        <v>79</v>
+      </c>
+      <c r="D43">
+        <v>6</v>
+      </c>
+      <c r="E43">
+        <v>2</v>
+      </c>
+      <c r="F43" t="s">
+        <v>21</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+      <c r="H43">
+        <v>5</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>75</v>
+      </c>
+      <c r="B44" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" t="s">
+        <v>79</v>
+      </c>
+      <c r="D44">
+        <v>3</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="F44" t="s">
+        <v>60</v>
+      </c>
+      <c r="G44">
+        <v>2</v>
+      </c>
+      <c r="H44">
+        <v>1</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>76</v>
+      </c>
+      <c r="B45" t="s">
+        <v>10</v>
+      </c>
+      <c r="C45" t="s">
+        <v>79</v>
+      </c>
+      <c r="D45">
+        <v>4</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="F45" t="s">
+        <v>60</v>
+      </c>
+      <c r="G45">
+        <v>2</v>
+      </c>
+      <c r="H45">
+        <v>3</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>77</v>
+      </c>
+      <c r="B46" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46" t="s">
+        <v>79</v>
+      </c>
+      <c r="D46">
+        <v>5</v>
+      </c>
+      <c r="E46">
+        <v>2</v>
+      </c>
+      <c r="F46" t="s">
+        <v>21</v>
+      </c>
+      <c r="G46">
+        <v>3</v>
+      </c>
+      <c r="H46">
+        <v>3</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>78</v>
+      </c>
+      <c r="B47" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" t="s">
+        <v>79</v>
+      </c>
+      <c r="D47">
+        <v>4</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47" t="s">
+        <v>21</v>
+      </c>
+      <c r="G47">
+        <v>3</v>
+      </c>
+      <c r="H47">
+        <v>3</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="J47" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added easy replay battle testing for better proof that it works
</commit_message>
<xml_diff>
--- a/cards.xlsx
+++ b/cards.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AustinWilliams\PycharmProjects\SPS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\PycharmProjects\SplinterlandsAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{892D20B2-707F-4F61-9A26-B81A7536E49A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F27AED-F5AB-4856-83CE-DC15CBE11191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4480" yWindow="1450" windowWidth="14400" windowHeight="9240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="146">
   <si>
     <t>Card</t>
   </si>
@@ -329,6 +329,135 @@
   </si>
   <si>
     <t>AttackType</t>
+  </si>
+  <si>
+    <t>Divine Healer</t>
+  </si>
+  <si>
+    <t>Feral Spirit</t>
+  </si>
+  <si>
+    <t>Silvershield Knight</t>
+  </si>
+  <si>
+    <t>Silvershield Warrior</t>
+  </si>
+  <si>
+    <t>Cave Slug</t>
+  </si>
+  <si>
+    <t>Crystal Jaguar</t>
+  </si>
+  <si>
+    <t>Lone Boatman</t>
+  </si>
+  <si>
+    <t>Herbalist</t>
+  </si>
+  <si>
+    <t>Tyrus Paladium</t>
+  </si>
+  <si>
+    <t>Peacebringer</t>
+  </si>
+  <si>
+    <t>Silvershield Paladin</t>
+  </si>
+  <si>
+    <t>Clay Golem</t>
+  </si>
+  <si>
+    <t>Truthspeaker</t>
+  </si>
+  <si>
+    <t>Luminous Eagle</t>
+  </si>
+  <si>
+    <t>Shieldbearer</t>
+  </si>
+  <si>
+    <t>Mother Khala</t>
+  </si>
+  <si>
+    <t>life</t>
+  </si>
+  <si>
+    <t>inspire</t>
+  </si>
+  <si>
+    <t>armor+</t>
+  </si>
+  <si>
+    <t>protect</t>
+  </si>
+  <si>
+    <t>taunt</t>
+  </si>
+  <si>
+    <t>Animated Corpse</t>
+  </si>
+  <si>
+    <t>Haunted Spider</t>
+  </si>
+  <si>
+    <t>Skeleton Assassin</t>
+  </si>
+  <si>
+    <t>Spineback Wolf</t>
+  </si>
+  <si>
+    <t>Maggots</t>
+  </si>
+  <si>
+    <t>Cursed Slimeball</t>
+  </si>
+  <si>
+    <t>Giant Scorpion</t>
+  </si>
+  <si>
+    <t>Undead Badger</t>
+  </si>
+  <si>
+    <t>Zintar Mortalis</t>
+  </si>
+  <si>
+    <t>Haunted Spirit</t>
+  </si>
+  <si>
+    <t>Twisted Jester</t>
+  </si>
+  <si>
+    <t>Undead Priest</t>
+  </si>
+  <si>
+    <t>Dark Astronomer</t>
+  </si>
+  <si>
+    <t>Bone Golem</t>
+  </si>
+  <si>
+    <t>Death Elemental</t>
+  </si>
+  <si>
+    <t>Contessa L'ament</t>
+  </si>
+  <si>
+    <t>Drake of Arnak</t>
+  </si>
+  <si>
+    <t>Naga Assassin</t>
+  </si>
+  <si>
+    <t>death</t>
+  </si>
+  <si>
+    <t>dragon</t>
+  </si>
+  <si>
+    <t>melee-</t>
+  </si>
+  <si>
+    <t>ranged-</t>
   </si>
 </sst>
 </file>
@@ -730,21 +859,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K63"/>
+  <dimension ref="A1:K97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E84" sqref="E84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.26953125" customWidth="1"/>
-    <col min="2" max="2" width="10.7265625" customWidth="1"/>
-    <col min="6" max="6" width="16.08984375" customWidth="1"/>
-    <col min="10" max="10" width="11.1796875" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -779,7 +908,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -808,7 +937,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -843,7 +972,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -875,7 +1004,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -907,7 +1036,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -936,7 +1065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -968,7 +1097,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1000,7 +1129,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -1029,7 +1158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -1061,7 +1190,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -1093,7 +1222,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -1125,7 +1254,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -1157,7 +1286,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -1189,7 +1318,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -1221,7 +1350,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -1250,7 +1379,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -1279,7 +1408,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -1311,7 +1440,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -1340,7 +1469,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>44</v>
       </c>
@@ -1369,7 +1498,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>45</v>
       </c>
@@ -1401,7 +1530,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>46</v>
       </c>
@@ -1433,7 +1562,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>47</v>
       </c>
@@ -1462,7 +1591,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>48</v>
       </c>
@@ -1491,7 +1620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>49</v>
       </c>
@@ -1523,7 +1652,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>50</v>
       </c>
@@ -1552,7 +1681,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>51</v>
       </c>
@@ -1581,7 +1710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>52</v>
       </c>
@@ -1613,7 +1742,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>53</v>
       </c>
@@ -1645,7 +1774,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>54</v>
       </c>
@@ -1677,7 +1806,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>55</v>
       </c>
@@ -1706,7 +1835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>56</v>
       </c>
@@ -1738,7 +1867,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>57</v>
       </c>
@@ -1767,7 +1896,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>63</v>
       </c>
@@ -1793,7 +1922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>64</v>
       </c>
@@ -1825,7 +1954,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>65</v>
       </c>
@@ -1857,7 +1986,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>66</v>
       </c>
@@ -1889,7 +2018,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>67</v>
       </c>
@@ -1918,7 +2047,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>68</v>
       </c>
@@ -1950,7 +2079,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>69</v>
       </c>
@@ -1982,7 +2111,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>70</v>
       </c>
@@ -2014,7 +2143,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>71</v>
       </c>
@@ -2046,7 +2175,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>72</v>
       </c>
@@ -2075,7 +2204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>73</v>
       </c>
@@ -2107,7 +2236,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>74</v>
       </c>
@@ -2136,7 +2265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>75</v>
       </c>
@@ -2165,7 +2294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>76</v>
       </c>
@@ -2197,7 +2326,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>79</v>
       </c>
@@ -2226,7 +2355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>80</v>
       </c>
@@ -2258,7 +2387,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>81</v>
       </c>
@@ -2287,7 +2416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>82</v>
       </c>
@@ -2319,7 +2448,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>83</v>
       </c>
@@ -2351,7 +2480,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>84</v>
       </c>
@@ -2380,7 +2509,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>85</v>
       </c>
@@ -2409,7 +2538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>86</v>
       </c>
@@ -2441,7 +2570,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>87</v>
       </c>
@@ -2470,7 +2599,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>88</v>
       </c>
@@ -2499,7 +2628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>89</v>
       </c>
@@ -2531,7 +2660,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>90</v>
       </c>
@@ -2563,7 +2692,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>91</v>
       </c>
@@ -2592,7 +2721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>96</v>
       </c>
@@ -2624,7 +2753,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>97</v>
       </c>
@@ -2656,7 +2785,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>98</v>
       </c>
@@ -2683,6 +2812,1046 @@
       </c>
       <c r="J63" t="s">
         <v>100</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>103</v>
+      </c>
+      <c r="B64" t="s">
+        <v>8</v>
+      </c>
+      <c r="C64" t="s">
+        <v>119</v>
+      </c>
+      <c r="D64">
+        <v>3</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="G64">
+        <v>1</v>
+      </c>
+      <c r="H64">
+        <v>4</v>
+      </c>
+      <c r="I64">
+        <v>0</v>
+      </c>
+      <c r="J64" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>104</v>
+      </c>
+      <c r="B65" t="s">
+        <v>8</v>
+      </c>
+      <c r="C65" t="s">
+        <v>119</v>
+      </c>
+      <c r="D65">
+        <v>3</v>
+      </c>
+      <c r="E65">
+        <v>1</v>
+      </c>
+      <c r="F65" t="s">
+        <v>10</v>
+      </c>
+      <c r="G65">
+        <v>4</v>
+      </c>
+      <c r="H65">
+        <v>2</v>
+      </c>
+      <c r="I65">
+        <v>0</v>
+      </c>
+      <c r="J65" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>105</v>
+      </c>
+      <c r="B66" t="s">
+        <v>8</v>
+      </c>
+      <c r="C66" t="s">
+        <v>119</v>
+      </c>
+      <c r="D66">
+        <v>6</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+      <c r="F66" t="s">
+        <v>10</v>
+      </c>
+      <c r="G66">
+        <v>4</v>
+      </c>
+      <c r="H66">
+        <v>5</v>
+      </c>
+      <c r="I66">
+        <v>1</v>
+      </c>
+      <c r="J66" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>106</v>
+      </c>
+      <c r="B67" t="s">
+        <v>8</v>
+      </c>
+      <c r="C67" t="s">
+        <v>119</v>
+      </c>
+      <c r="D67">
+        <v>4</v>
+      </c>
+      <c r="E67">
+        <v>1</v>
+      </c>
+      <c r="F67" t="s">
+        <v>10</v>
+      </c>
+      <c r="G67">
+        <v>1</v>
+      </c>
+      <c r="H67">
+        <v>3</v>
+      </c>
+      <c r="I67">
+        <v>1</v>
+      </c>
+      <c r="J67" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>107</v>
+      </c>
+      <c r="B68" t="s">
+        <v>8</v>
+      </c>
+      <c r="C68" t="s">
+        <v>119</v>
+      </c>
+      <c r="D68">
+        <v>5</v>
+      </c>
+      <c r="E68">
+        <v>2</v>
+      </c>
+      <c r="F68" t="s">
+        <v>10</v>
+      </c>
+      <c r="G68">
+        <v>1</v>
+      </c>
+      <c r="H68">
+        <v>4</v>
+      </c>
+      <c r="I68">
+        <v>0</v>
+      </c>
+      <c r="J68" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>108</v>
+      </c>
+      <c r="B69" t="s">
+        <v>8</v>
+      </c>
+      <c r="C69" t="s">
+        <v>119</v>
+      </c>
+      <c r="D69">
+        <v>4</v>
+      </c>
+      <c r="E69">
+        <v>1</v>
+      </c>
+      <c r="F69" t="s">
+        <v>10</v>
+      </c>
+      <c r="G69">
+        <v>2</v>
+      </c>
+      <c r="H69">
+        <v>5</v>
+      </c>
+      <c r="I69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>109</v>
+      </c>
+      <c r="B70" t="s">
+        <v>8</v>
+      </c>
+      <c r="C70" t="s">
+        <v>119</v>
+      </c>
+      <c r="D70">
+        <v>5</v>
+      </c>
+      <c r="E70">
+        <v>2</v>
+      </c>
+      <c r="F70" t="s">
+        <v>19</v>
+      </c>
+      <c r="G70">
+        <v>2</v>
+      </c>
+      <c r="H70">
+        <v>3</v>
+      </c>
+      <c r="I70">
+        <v>1</v>
+      </c>
+      <c r="J70" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>110</v>
+      </c>
+      <c r="B71" t="s">
+        <v>8</v>
+      </c>
+      <c r="C71" t="s">
+        <v>119</v>
+      </c>
+      <c r="D71">
+        <v>2</v>
+      </c>
+      <c r="E71">
+        <v>1</v>
+      </c>
+      <c r="F71" t="s">
+        <v>19</v>
+      </c>
+      <c r="G71">
+        <v>1</v>
+      </c>
+      <c r="H71">
+        <v>2</v>
+      </c>
+      <c r="I71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>111</v>
+      </c>
+      <c r="B72" t="s">
+        <v>38</v>
+      </c>
+      <c r="C72" t="s">
+        <v>119</v>
+      </c>
+      <c r="D72">
+        <v>3</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="G72">
+        <v>0</v>
+      </c>
+      <c r="H72">
+        <v>0</v>
+      </c>
+      <c r="I72">
+        <v>0</v>
+      </c>
+      <c r="J72" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>112</v>
+      </c>
+      <c r="B73" t="s">
+        <v>8</v>
+      </c>
+      <c r="C73" t="s">
+        <v>119</v>
+      </c>
+      <c r="D73">
+        <v>4</v>
+      </c>
+      <c r="E73">
+        <v>2</v>
+      </c>
+      <c r="F73" t="s">
+        <v>19</v>
+      </c>
+      <c r="G73">
+        <v>3</v>
+      </c>
+      <c r="H73">
+        <v>4</v>
+      </c>
+      <c r="I73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>113</v>
+      </c>
+      <c r="B74" t="s">
+        <v>8</v>
+      </c>
+      <c r="C74" t="s">
+        <v>119</v>
+      </c>
+      <c r="D74">
+        <v>5</v>
+      </c>
+      <c r="E74">
+        <v>1</v>
+      </c>
+      <c r="F74" t="s">
+        <v>10</v>
+      </c>
+      <c r="G74">
+        <v>2</v>
+      </c>
+      <c r="H74">
+        <v>5</v>
+      </c>
+      <c r="I74">
+        <v>1</v>
+      </c>
+      <c r="J74" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>114</v>
+      </c>
+      <c r="B75" t="s">
+        <v>8</v>
+      </c>
+      <c r="C75" t="s">
+        <v>119</v>
+      </c>
+      <c r="D75">
+        <v>6</v>
+      </c>
+      <c r="E75">
+        <v>3</v>
+      </c>
+      <c r="F75" t="s">
+        <v>10</v>
+      </c>
+      <c r="G75">
+        <v>1</v>
+      </c>
+      <c r="H75">
+        <v>7</v>
+      </c>
+      <c r="I75">
+        <v>0</v>
+      </c>
+      <c r="J75" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>115</v>
+      </c>
+      <c r="B76" t="s">
+        <v>8</v>
+      </c>
+      <c r="C76" t="s">
+        <v>119</v>
+      </c>
+      <c r="D76">
+        <v>3</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+      <c r="G76">
+        <v>2</v>
+      </c>
+      <c r="H76">
+        <v>1</v>
+      </c>
+      <c r="I76">
+        <v>0</v>
+      </c>
+      <c r="J76" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>116</v>
+      </c>
+      <c r="B77" t="s">
+        <v>8</v>
+      </c>
+      <c r="C77" t="s">
+        <v>119</v>
+      </c>
+      <c r="D77">
+        <v>6</v>
+      </c>
+      <c r="E77">
+        <v>2</v>
+      </c>
+      <c r="F77" t="s">
+        <v>10</v>
+      </c>
+      <c r="G77">
+        <v>3</v>
+      </c>
+      <c r="H77">
+        <v>5</v>
+      </c>
+      <c r="I77">
+        <v>0</v>
+      </c>
+      <c r="J77" t="s">
+        <v>23</v>
+      </c>
+      <c r="K77" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>117</v>
+      </c>
+      <c r="B78" t="s">
+        <v>8</v>
+      </c>
+      <c r="C78" t="s">
+        <v>119</v>
+      </c>
+      <c r="D78">
+        <v>8</v>
+      </c>
+      <c r="E78">
+        <v>2</v>
+      </c>
+      <c r="F78" t="s">
+        <v>10</v>
+      </c>
+      <c r="G78">
+        <v>2</v>
+      </c>
+      <c r="H78">
+        <v>9</v>
+      </c>
+      <c r="I78">
+        <v>4</v>
+      </c>
+      <c r="J78" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>118</v>
+      </c>
+      <c r="B79" t="s">
+        <v>38</v>
+      </c>
+      <c r="C79" t="s">
+        <v>119</v>
+      </c>
+      <c r="D79">
+        <v>3</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+      <c r="G79">
+        <v>0</v>
+      </c>
+      <c r="H79">
+        <v>0</v>
+      </c>
+      <c r="I79">
+        <v>0</v>
+      </c>
+      <c r="J79" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>124</v>
+      </c>
+      <c r="B80" t="s">
+        <v>8</v>
+      </c>
+      <c r="C80" t="s">
+        <v>142</v>
+      </c>
+      <c r="D80">
+        <v>4</v>
+      </c>
+      <c r="E80">
+        <v>2</v>
+      </c>
+      <c r="F80" t="s">
+        <v>10</v>
+      </c>
+      <c r="G80">
+        <v>1</v>
+      </c>
+      <c r="H80">
+        <v>6</v>
+      </c>
+      <c r="I80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>125</v>
+      </c>
+      <c r="B81" t="s">
+        <v>8</v>
+      </c>
+      <c r="C81" t="s">
+        <v>142</v>
+      </c>
+      <c r="D81">
+        <v>3</v>
+      </c>
+      <c r="E81">
+        <v>2</v>
+      </c>
+      <c r="F81" t="s">
+        <v>19</v>
+      </c>
+      <c r="G81">
+        <v>1</v>
+      </c>
+      <c r="H81">
+        <v>2</v>
+      </c>
+      <c r="I81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>126</v>
+      </c>
+      <c r="B82" t="s">
+        <v>8</v>
+      </c>
+      <c r="C82" t="s">
+        <v>142</v>
+      </c>
+      <c r="D82">
+        <v>3</v>
+      </c>
+      <c r="E82">
+        <v>1</v>
+      </c>
+      <c r="F82" t="s">
+        <v>10</v>
+      </c>
+      <c r="G82">
+        <v>4</v>
+      </c>
+      <c r="H82">
+        <v>2</v>
+      </c>
+      <c r="I82">
+        <v>0</v>
+      </c>
+      <c r="J82" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>127</v>
+      </c>
+      <c r="B83" t="s">
+        <v>8</v>
+      </c>
+      <c r="C83" t="s">
+        <v>142</v>
+      </c>
+      <c r="D83">
+        <v>5</v>
+      </c>
+      <c r="E83">
+        <v>1</v>
+      </c>
+      <c r="F83" t="s">
+        <v>10</v>
+      </c>
+      <c r="G83">
+        <v>6</v>
+      </c>
+      <c r="H83">
+        <v>3</v>
+      </c>
+      <c r="I83">
+        <v>1</v>
+      </c>
+      <c r="J83" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>128</v>
+      </c>
+      <c r="B84" t="s">
+        <v>8</v>
+      </c>
+      <c r="C84" t="s">
+        <v>142</v>
+      </c>
+      <c r="D84">
+        <v>3</v>
+      </c>
+      <c r="E84">
+        <v>1</v>
+      </c>
+      <c r="F84" t="s">
+        <v>10</v>
+      </c>
+      <c r="G84">
+        <v>1</v>
+      </c>
+      <c r="H84">
+        <v>1</v>
+      </c>
+      <c r="I84">
+        <v>0</v>
+      </c>
+      <c r="J84" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>129</v>
+      </c>
+      <c r="B85" t="s">
+        <v>8</v>
+      </c>
+      <c r="C85" t="s">
+        <v>142</v>
+      </c>
+      <c r="D85">
+        <v>1</v>
+      </c>
+      <c r="E85">
+        <v>1</v>
+      </c>
+      <c r="F85" t="s">
+        <v>10</v>
+      </c>
+      <c r="G85">
+        <v>1</v>
+      </c>
+      <c r="H85">
+        <v>1</v>
+      </c>
+      <c r="I85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>130</v>
+      </c>
+      <c r="B86" t="s">
+        <v>8</v>
+      </c>
+      <c r="C86" t="s">
+        <v>142</v>
+      </c>
+      <c r="D86">
+        <v>4</v>
+      </c>
+      <c r="E86">
+        <v>1</v>
+      </c>
+      <c r="F86" t="s">
+        <v>10</v>
+      </c>
+      <c r="G86">
+        <v>2</v>
+      </c>
+      <c r="H86">
+        <v>4</v>
+      </c>
+      <c r="I86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>131</v>
+      </c>
+      <c r="B87" t="s">
+        <v>8</v>
+      </c>
+      <c r="C87" t="s">
+        <v>142</v>
+      </c>
+      <c r="D87">
+        <v>2</v>
+      </c>
+      <c r="E87">
+        <v>1</v>
+      </c>
+      <c r="F87" t="s">
+        <v>10</v>
+      </c>
+      <c r="G87">
+        <v>3</v>
+      </c>
+      <c r="H87">
+        <v>1</v>
+      </c>
+      <c r="I87">
+        <v>0</v>
+      </c>
+      <c r="J87" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>132</v>
+      </c>
+      <c r="B88" t="s">
+        <v>38</v>
+      </c>
+      <c r="C88" t="s">
+        <v>142</v>
+      </c>
+      <c r="D88">
+        <v>3</v>
+      </c>
+      <c r="E88">
+        <v>0</v>
+      </c>
+      <c r="G88">
+        <v>0</v>
+      </c>
+      <c r="H88">
+        <v>0</v>
+      </c>
+      <c r="I88">
+        <v>0</v>
+      </c>
+      <c r="J88" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>133</v>
+      </c>
+      <c r="B89" t="s">
+        <v>8</v>
+      </c>
+      <c r="C89" t="s">
+        <v>142</v>
+      </c>
+      <c r="D89">
+        <v>5</v>
+      </c>
+      <c r="E89">
+        <v>2</v>
+      </c>
+      <c r="F89" t="s">
+        <v>10</v>
+      </c>
+      <c r="G89">
+        <v>2</v>
+      </c>
+      <c r="H89">
+        <v>7</v>
+      </c>
+      <c r="I89">
+        <v>0</v>
+      </c>
+      <c r="J89" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>134</v>
+      </c>
+      <c r="B90" t="s">
+        <v>8</v>
+      </c>
+      <c r="C90" t="s">
+        <v>142</v>
+      </c>
+      <c r="D90">
+        <v>4</v>
+      </c>
+      <c r="E90">
+        <v>2</v>
+      </c>
+      <c r="F90" t="s">
+        <v>19</v>
+      </c>
+      <c r="G90">
+        <v>3</v>
+      </c>
+      <c r="H90">
+        <v>4</v>
+      </c>
+      <c r="I90">
+        <v>0</v>
+      </c>
+      <c r="J90" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>135</v>
+      </c>
+      <c r="B91" t="s">
+        <v>8</v>
+      </c>
+      <c r="C91" t="s">
+        <v>142</v>
+      </c>
+      <c r="D91">
+        <v>2</v>
+      </c>
+      <c r="E91">
+        <v>0</v>
+      </c>
+      <c r="G91">
+        <v>1</v>
+      </c>
+      <c r="H91">
+        <v>3</v>
+      </c>
+      <c r="I91">
+        <v>0</v>
+      </c>
+      <c r="J91" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>136</v>
+      </c>
+      <c r="B92" t="s">
+        <v>8</v>
+      </c>
+      <c r="C92" t="s">
+        <v>142</v>
+      </c>
+      <c r="D92">
+        <v>4</v>
+      </c>
+      <c r="E92">
+        <v>2</v>
+      </c>
+      <c r="F92" t="s">
+        <v>19</v>
+      </c>
+      <c r="G92">
+        <v>1</v>
+      </c>
+      <c r="H92">
+        <v>4</v>
+      </c>
+      <c r="I92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>137</v>
+      </c>
+      <c r="B93" t="s">
+        <v>8</v>
+      </c>
+      <c r="C93" t="s">
+        <v>142</v>
+      </c>
+      <c r="D93">
+        <v>7</v>
+      </c>
+      <c r="E93">
+        <v>3</v>
+      </c>
+      <c r="F93" t="s">
+        <v>10</v>
+      </c>
+      <c r="G93">
+        <v>1</v>
+      </c>
+      <c r="H93">
+        <v>6</v>
+      </c>
+      <c r="I93">
+        <v>2</v>
+      </c>
+      <c r="J93" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>138</v>
+      </c>
+      <c r="B94" t="s">
+        <v>8</v>
+      </c>
+      <c r="C94" t="s">
+        <v>142</v>
+      </c>
+      <c r="D94">
+        <v>3</v>
+      </c>
+      <c r="E94">
+        <v>1</v>
+      </c>
+      <c r="F94" t="s">
+        <v>58</v>
+      </c>
+      <c r="G94">
+        <v>3</v>
+      </c>
+      <c r="H94">
+        <v>2</v>
+      </c>
+      <c r="I94">
+        <v>0</v>
+      </c>
+      <c r="J94" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>139</v>
+      </c>
+      <c r="B95" t="s">
+        <v>38</v>
+      </c>
+      <c r="C95" t="s">
+        <v>142</v>
+      </c>
+      <c r="D95">
+        <v>3</v>
+      </c>
+      <c r="E95">
+        <v>0</v>
+      </c>
+      <c r="G95">
+        <v>0</v>
+      </c>
+      <c r="H95">
+        <v>0</v>
+      </c>
+      <c r="I95">
+        <v>0</v>
+      </c>
+      <c r="J95" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>140</v>
+      </c>
+      <c r="B96" t="s">
+        <v>38</v>
+      </c>
+      <c r="C96" t="s">
+        <v>143</v>
+      </c>
+      <c r="D96">
+        <v>4</v>
+      </c>
+      <c r="E96">
+        <v>0</v>
+      </c>
+      <c r="G96">
+        <v>0</v>
+      </c>
+      <c r="H96">
+        <v>0</v>
+      </c>
+      <c r="I96">
+        <v>0</v>
+      </c>
+      <c r="J96" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>141</v>
+      </c>
+      <c r="B97" t="s">
+        <v>8</v>
+      </c>
+      <c r="C97" t="s">
+        <v>143</v>
+      </c>
+      <c r="D97">
+        <v>2</v>
+      </c>
+      <c r="E97">
+        <v>1</v>
+      </c>
+      <c r="F97" t="s">
+        <v>19</v>
+      </c>
+      <c r="G97">
+        <v>5</v>
+      </c>
+      <c r="H97">
+        <v>2</v>
+      </c>
+      <c r="I97">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added command line parsing
</commit_message>
<xml_diff>
--- a/cards.xlsx
+++ b/cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\PycharmProjects\SplinterlandsAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F27AED-F5AB-4856-83CE-DC15CBE11191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{704D900A-1010-4870-B051-B7B9F6184746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3255" yWindow="2490" windowWidth="28800" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="147">
   <si>
     <t>Card</t>
   </si>
@@ -458,6 +458,9 @@
   </si>
   <si>
     <t>ranged-</t>
+  </si>
+  <si>
+    <t>none</t>
   </si>
 </sst>
 </file>
@@ -861,8 +864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E84" sqref="E84"/>
+    <sheetView tabSelected="1" topLeftCell="C64" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G91" sqref="G91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -924,6 +927,9 @@
       <c r="E2">
         <v>0</v>
       </c>
+      <c r="F2" t="s">
+        <v>146</v>
+      </c>
       <c r="G2">
         <v>2</v>
       </c>
@@ -1366,6 +1372,9 @@
       <c r="E16">
         <v>0</v>
       </c>
+      <c r="F16" t="s">
+        <v>146</v>
+      </c>
       <c r="G16">
         <v>0</v>
       </c>
@@ -1395,6 +1404,9 @@
       <c r="E17">
         <v>0</v>
       </c>
+      <c r="F17" t="s">
+        <v>146</v>
+      </c>
       <c r="G17">
         <v>0</v>
       </c>
@@ -1485,6 +1497,9 @@
       <c r="E20">
         <v>0</v>
       </c>
+      <c r="F20" t="s">
+        <v>146</v>
+      </c>
       <c r="G20">
         <v>1</v>
       </c>
@@ -1578,6 +1593,9 @@
       <c r="E23">
         <v>0</v>
       </c>
+      <c r="F23" t="s">
+        <v>146</v>
+      </c>
       <c r="G23">
         <v>1</v>
       </c>
@@ -1668,6 +1686,9 @@
       <c r="E26">
         <v>0</v>
       </c>
+      <c r="F26" t="s">
+        <v>146</v>
+      </c>
       <c r="G26">
         <v>0</v>
       </c>
@@ -1883,6 +1904,9 @@
       <c r="E33">
         <v>0</v>
       </c>
+      <c r="F33" t="s">
+        <v>146</v>
+      </c>
       <c r="G33">
         <v>0</v>
       </c>
@@ -1912,6 +1936,9 @@
       <c r="E34">
         <v>0</v>
       </c>
+      <c r="F34" t="s">
+        <v>146</v>
+      </c>
       <c r="G34">
         <v>1</v>
       </c>
@@ -2496,6 +2523,9 @@
       <c r="E53">
         <v>0</v>
       </c>
+      <c r="F53" t="s">
+        <v>146</v>
+      </c>
       <c r="G53">
         <v>2</v>
       </c>
@@ -2586,6 +2616,9 @@
       <c r="E56">
         <v>0</v>
       </c>
+      <c r="F56" t="s">
+        <v>146</v>
+      </c>
       <c r="G56">
         <v>0</v>
       </c>
@@ -2801,6 +2834,9 @@
       <c r="E63">
         <v>0</v>
       </c>
+      <c r="F63" t="s">
+        <v>146</v>
+      </c>
       <c r="G63">
         <v>0</v>
       </c>
@@ -2830,6 +2866,9 @@
       <c r="E64">
         <v>0</v>
       </c>
+      <c r="F64" t="s">
+        <v>146</v>
+      </c>
       <c r="G64">
         <v>1</v>
       </c>
@@ -3077,6 +3116,9 @@
       <c r="E72">
         <v>0</v>
       </c>
+      <c r="F72" t="s">
+        <v>146</v>
+      </c>
       <c r="G72">
         <v>0</v>
       </c>
@@ -3199,6 +3241,9 @@
       <c r="E76">
         <v>0</v>
       </c>
+      <c r="F76" t="s">
+        <v>146</v>
+      </c>
       <c r="G76">
         <v>2</v>
       </c>
@@ -3295,6 +3340,9 @@
       <c r="E79">
         <v>0</v>
       </c>
+      <c r="F79" t="s">
+        <v>146</v>
+      </c>
       <c r="G79">
         <v>0</v>
       </c>
@@ -3568,6 +3616,9 @@
       <c r="E88">
         <v>0</v>
       </c>
+      <c r="F88" t="s">
+        <v>146</v>
+      </c>
       <c r="G88">
         <v>0</v>
       </c>
@@ -3661,6 +3712,9 @@
       <c r="E91">
         <v>0</v>
       </c>
+      <c r="F91" t="s">
+        <v>146</v>
+      </c>
       <c r="G91">
         <v>1</v>
       </c>
@@ -3783,6 +3837,9 @@
       <c r="E95">
         <v>0</v>
       </c>
+      <c r="F95" t="s">
+        <v>146</v>
+      </c>
       <c r="G95">
         <v>0</v>
       </c>
@@ -3811,6 +3868,9 @@
       </c>
       <c r="E96">
         <v>0</v>
+      </c>
+      <c r="F96" t="s">
+        <v>146</v>
       </c>
       <c r="G96">
         <v>0</v>

</xml_diff>